<commit_message>
collect first batch of kobe videos
</commit_message>
<xml_diff>
--- a/kobe_videos.xlsx
+++ b/kobe_videos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,17 +461,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>vpI0tk9G2Jc</t>
+          <t>lk5o2PK76hs</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2022-01-26 13:00:36 +0000</t>
+          <t>2010-10-28T21:49:10Z</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=vpI0tk9G2Jc</t>
+          <t>https://www.youtube.com/watch?v=lk5o2PK76hs</t>
         </is>
       </c>
     </row>
@@ -481,17 +481,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>JqGCDusQE-8</t>
+          <t>cU63znm-aO8</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2014-10-22 00:52:25 +0000</t>
+          <t>2011-12-30T07:24:03Z</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=JqGCDusQE-8</t>
+          <t>https://www.youtube.com/watch?v=cU63znm-aO8</t>
         </is>
       </c>
     </row>
@@ -501,17 +501,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>OheQLsSRjTk</t>
+          <t>xXtA4QTfKT8</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2018-08-20 18:47:04 +0000</t>
+          <t>2019-09-08T14:17:19Z</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=OheQLsSRjTk</t>
+          <t>https://www.youtube.com/watch?v=xXtA4QTfKT8</t>
         </is>
       </c>
     </row>
@@ -521,17 +521,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>FeXZY4eVLlo</t>
+          <t>ZyBDKu55EGw</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2008-01-22 16:05:15 +0000</t>
+          <t>2020-05-07T15:18:10Z</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=FeXZY4eVLlo</t>
+          <t>https://www.youtube.com/watch?v=ZyBDKu55EGw</t>
         </is>
       </c>
     </row>
@@ -541,17 +541,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>rPeOm3JnVOY</t>
+          <t>HbaarPJ3Jvs</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2014-10-04 10:17:35 +0000</t>
+          <t>2016-05-18T22:47:36Z</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=rPeOm3JnVOY</t>
+          <t>https://www.youtube.com/watch?v=HbaarPJ3Jvs</t>
         </is>
       </c>
     </row>
@@ -561,17 +561,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>rrZnYJ3-R0c</t>
+          <t>qgHCnPoJ4wE</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2020-07-10 14:28:16 +0000</t>
+          <t>2022-03-17T20:14:04Z</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=rrZnYJ3-R0c</t>
+          <t>https://www.youtube.com/watch?v=qgHCnPoJ4wE</t>
         </is>
       </c>
     </row>
@@ -581,17 +581,717 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>L-jfb98i8ME</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2016-02-28T04:55:45Z</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=L-jfb98i8ME</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>kn3lul0Oee0</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2020-05-07T20:24:56Z</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=kn3lul0Oee0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MDWmwWdfrXc</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2013-04-09T19:14:51Z</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=MDWmwWdfrXc</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>FUYSSDj_ntg</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2018-08-23T20:00:01Z</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=FUYSSDj_ntg</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>gIqhVfsB1n8</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2015-08-29T20:09:18Z</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=gIqhVfsB1n8</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Rx2inwUj_F0</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2016-04-15T16:50:10Z</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=Rx2inwUj_F0</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>pKTLxG0wGfg</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2019-01-29T02:45:00Z</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=pKTLxG0wGfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>T6UnitdiLo0</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2015-11-30T15:04:36Z</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=T6UnitdiLo0</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>VRu4GIZLtb4</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2015-11-10T21:12:32Z</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=VRu4GIZLtb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Zw7Qxy6aKeY</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2018-05-16T16:00:30Z</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=Zw7Qxy6aKeY</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Q8BSoh6qAY4</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2019-02-17T17:00:02Z</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=Q8BSoh6qAY4</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>FeXZY4eVLlo</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2008-01-22T16:05:15Z</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=FeXZY4eVLlo</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>l6L3fqXxVYs</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2021-11-27T04:00:10Z</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=l6L3fqXxVYs</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>cGBI6PvPznA</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2009-06-05 05:56:09 +0000</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2009-06-05T05:56:09Z</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
         <is>
           <t>https://www.youtube.com/watch?v=cGBI6PvPznA</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>1fjhIWJSxfw</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2018-08-23T16:00:01Z</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=1fjhIWJSxfw</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>adRunnK0muY</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2022-12-10T00:30:45Z</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=adRunnK0muY</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>rrZnYJ3-R0c</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2020-07-10T14:28:16Z</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=rrZnYJ3-R0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>a9MfQKnvEkk</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2014-08-28T20:02:59Z</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=a9MfQKnvEkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>x3sTzWCvk5o</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2020-05-21T18:39:46Z</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=x3sTzWCvk5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>fhpVE5Yfvhc</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2011-10-25T07:39:02Z</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=fhpVE5Yfvhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>1vzBFmRYyE0</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2019-08-24T14:30:00Z</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=1vzBFmRYyE0</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Us5QIvuahx4</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2010-11-25T00:24:23Z</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=Us5QIvuahx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>A2JE2L4vhNA</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2013-03-09T08:30:26Z</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=A2JE2L4vhNA</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>t9jmWZ6u-44</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2022-08-23T22:14:40Z</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=t9jmWZ6u-44</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>xXtA4QTfKT8</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2019-09-08T14:17:19Z</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=xXtA4QTfKT8</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SgCiqocx6WQ</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2016-04-17T20:44:34Z</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=SgCiqocx6WQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2JjjXPT0IPQ</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2016-09-10T00:13:38Z</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=2JjjXPT0IPQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>gzIS-RiKckM</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2017-05-14T14:13:00Z</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=gzIS-RiKckM</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>UhfbDpETimU</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2020-07-09T20:40:12Z</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=UhfbDpETimU</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>3sYuZ6Oftfk</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2018-03-05T22:28:18Z</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=3sYuZ6Oftfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>KfgNROlaIE4</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2017-09-22T10:53:41Z</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=KfgNROlaIE4</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>lD72I6MLqao</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2021-08-28T08:12:55Z</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=lD72I6MLqao</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>hrB11u4ZDas</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2019-06-20T05:22:02Z</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=hrB11u4ZDas</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>a9MfQKnvEkk</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2014-08-28T20:02:59Z</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=a9MfQKnvEkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>q9_dBKE2yCc</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2015-09-22T07:21:20Z</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=q9_dBKE2yCc</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>xGoCyf8FDoI</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2020-02-14T12:23:56Z</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=xGoCyf8FDoI</t>
         </is>
       </c>
     </row>

</xml_diff>